<commit_message>
working on person detection
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab993ec8c675cc6f/Fall 2020/Interactive Device Design/BugBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{D5F03140-C2BD-4C19-A979-7A767C288685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9BA99DEC-0C3C-4C77-97C8-4A6CE0555E2F}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{D5F03140-C2BD-4C19-A979-7A767C288685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7BDAD3C8-F62F-4E30-8A72-0A647E3D07F6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DC583A4B-1A58-4003-8B53-1793EC605AD0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Part</t>
   </si>
@@ -78,13 +78,19 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/3942</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +102,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,9 +136,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -440,25 +457,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F7A8DE-7BD9-4AF3-85B4-570DD44A22DC}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.7265625" style="3"/>
+    <col min="4" max="4" width="8.7265625" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
@@ -469,13 +490,13 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>9.9499999999999993</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <f>C2*B2</f>
         <v>9.9499999999999993</v>
       </c>
@@ -487,13 +508,13 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>4.95</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <f t="shared" ref="D3:D6" si="0">C3*B3</f>
         <v>4.95</v>
       </c>
@@ -505,13 +526,13 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1.95</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
         <v>1.95</v>
       </c>
@@ -523,13 +544,13 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>7.5</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -541,18 +562,27 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>3.95</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>3.95</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4">
+        <f>SUM(D2:D6)</f>
+        <v>35.799999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -564,5 +594,6 @@
     <hyperlink ref="E6" r:id="rId5" xr:uid="{B4349E1E-982F-4126-A266-BBCC6B46B339}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>